<commit_message>
feat: add tenant logo support and remove department field from employee management
</commit_message>
<xml_diff>
--- a/Onboard/selsfot/TimePulse_Client_Onoarding_Document (2).xlsx
+++ b/Onboard/selsfot/TimePulse_Client_Onoarding_Document (2).xlsx
@@ -1,19 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selva/Projects/TimePulse/Onboard/selsfot/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1980E8A-856A-104B-9E58-ABE0A5A91F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Client" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Users" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Employees" sheetId="3" r:id="rId6"/>
+    <sheet name="Client" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="2" r:id="rId2"/>
+    <sheet name="Employees" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>Legal Name</t>
   </si>
@@ -169,28 +190,41 @@
   </si>
   <si>
     <t xml:space="preserve">Lalitha </t>
+  </si>
+  <si>
+    <t>Phone Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -199,7 +233,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -209,43 +243,41 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -435,24 +467,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.13"/>
-    <col customWidth="1" min="2" max="2" width="19.63"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -480,10 +517,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="1">
-        <v>75002.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>75002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -500,18 +537,18 @@
         <v>7</v>
       </c>
       <c r="F5" s="1">
-        <v>75002.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>75002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>2.05521435E8</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>205521435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -522,7 +559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -530,7 +567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -538,25 +575,34 @@
         <v>16</v>
       </c>
     </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="19.63"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
@@ -573,7 +619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -590,7 +636,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
@@ -607,7 +653,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -621,7 +667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
@@ -638,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
@@ -652,7 +698,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -669,7 +715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
@@ -684,25 +730,28 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A3:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="20.25"/>
-    <col customWidth="1" min="5" max="5" width="22.25"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -722,12 +771,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>37</v>
@@ -742,12 +791,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>41</v>
@@ -762,12 +811,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>45</v>
@@ -782,12 +831,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
@@ -802,12 +851,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
@@ -822,12 +871,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>51</v>
@@ -842,12 +891,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>